<commit_message>
Update BOMS and add changelog describing the reason for the updates Add PDF with some assembly notes
</commit_message>
<xml_diff>
--- a/Gen1/Assembly/BOM_CSaAF.xlsx
+++ b/Gen1/Assembly/BOM_CSaAF.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14820"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_CSaAF" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="120">
   <si>
     <t>Qty</t>
   </si>
@@ -407,6 +407,24 @@
   </si>
   <si>
     <t>4-40 Standoffs to support NI-USb7856 with support board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Instruments 777584-01 </t>
+  </si>
+  <si>
+    <t>PS-2 Power  Supply for USB7856</t>
+  </si>
+  <si>
+    <t>National Instruments 196739-01</t>
+  </si>
+  <si>
+    <t>National Instruments 196375-01</t>
+  </si>
+  <si>
+    <t>NI 9976 2 Pos Terminal Block for USB7856 PS-2 Power Supply</t>
+  </si>
+  <si>
+    <t>Backshell for NI 9976 Terminal Block</t>
   </si>
 </sst>
 </file>
@@ -800,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,6 +884,39 @@
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>119</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
     </row>
@@ -884,7 +935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>

</xml_diff>